<commit_message>
get D_i,d_ij for optimization with many files
</commit_message>
<xml_diff>
--- a/Preprocess/goods_ij.xlsx
+++ b/Preprocess/goods_ij.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11290\Desktop\数模比赛\EXCEL表\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aaaStudy\MathModel_Optimization\Project\2023C\Preprocess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F602520D-5B49-43E8-BF88-E6A0D7E63A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20C15E-330E-49DA-B293-4FCB7009BB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="1545" windowWidth="20865" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1671,6 +1671,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1707,9 +1710,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2016,20 +2022,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I242" sqref="I242"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A237" sqref="A237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2048,8 +2054,8 @@
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>310</v>
       </c>
       <c r="B2" t="s">
@@ -2068,8 +2074,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B3" t="s">
@@ -2088,8 +2094,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B4" t="s">
@@ -2108,8 +2114,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B5" t="s">
@@ -2128,8 +2134,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
         <v>328</v>
       </c>
       <c r="B6" t="s">
@@ -2148,8 +2154,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>337</v>
       </c>
       <c r="B7" t="s">
@@ -2168,8 +2174,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B8" t="s">
@@ -2188,8 +2194,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>235</v>
       </c>
       <c r="B9" t="s">
@@ -2208,8 +2214,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B10" t="s">
@@ -2228,8 +2234,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>340</v>
       </c>
       <c r="B11" t="s">
@@ -2248,8 +2254,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B12" t="s">
@@ -2268,8 +2274,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B13" t="s">
@@ -2288,8 +2294,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B14" t="s">
@@ -2308,8 +2314,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
         <v>312</v>
       </c>
       <c r="B15" t="s">
@@ -2328,8 +2334,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
         <v>342</v>
       </c>
       <c r="B16" t="s">
@@ -2348,8 +2354,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
         <v>300</v>
       </c>
       <c r="B17" t="s">
@@ -2368,8 +2374,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B18" t="s">
@@ -2388,8 +2394,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
         <v>308</v>
       </c>
       <c r="B19" t="s">
@@ -2408,8 +2414,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B20" t="s">
@@ -2428,8 +2434,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B21" t="s">
@@ -2448,8 +2454,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B22" t="s">
@@ -2468,8 +2474,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B23" t="s">
@@ -2488,8 +2494,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B24" t="s">
@@ -2508,8 +2514,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B25" t="s">
@@ -2528,8 +2534,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B26" t="s">
@@ -2548,8 +2554,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B27" t="s">
@@ -2568,8 +2574,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B28" t="s">
@@ -2588,8 +2594,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B29" t="s">
@@ -2608,8 +2614,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B30" t="s">
@@ -2628,8 +2634,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="2" t="s">
         <v>219</v>
       </c>
       <c r="B31" t="s">
@@ -2648,8 +2654,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B32" t="s">
@@ -2668,8 +2674,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B33" t="s">
@@ -2688,8 +2694,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
         <v>223</v>
       </c>
       <c r="B34" t="s">
@@ -2708,8 +2714,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B35" t="s">
@@ -2728,8 +2734,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="2" t="s">
         <v>225</v>
       </c>
       <c r="B36" t="s">
@@ -2748,8 +2754,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B37" t="s">
@@ -2768,8 +2774,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B38" t="s">
@@ -2788,8 +2794,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="2" t="s">
         <v>316</v>
       </c>
       <c r="B39" t="s">
@@ -2808,8 +2814,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="2" t="s">
         <v>318</v>
       </c>
       <c r="B40" t="s">
@@ -2828,8 +2834,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
         <v>335</v>
       </c>
       <c r="B41" t="s">
@@ -2848,8 +2854,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B42" t="s">
@@ -2868,8 +2874,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B43" t="s">
@@ -2888,8 +2894,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="2" t="s">
         <v>322</v>
       </c>
       <c r="B44" t="s">
@@ -2908,8 +2914,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B45" t="s">
@@ -2928,8 +2934,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="2" t="s">
         <v>320</v>
       </c>
       <c r="B46" t="s">
@@ -2948,8 +2954,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="2" t="s">
         <v>239</v>
       </c>
       <c r="B47" t="s">
@@ -2968,8 +2974,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="2" t="s">
         <v>333</v>
       </c>
       <c r="B48" t="s">
@@ -2988,8 +2994,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" s="2" t="s">
         <v>241</v>
       </c>
       <c r="B49" t="s">
@@ -3008,8 +3014,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50" s="2" t="s">
         <v>243</v>
       </c>
       <c r="B50" t="s">
@@ -3028,8 +3034,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" s="2" t="s">
         <v>245</v>
       </c>
       <c r="B51" t="s">
@@ -3048,8 +3054,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
         <v>302</v>
       </c>
       <c r="B52" t="s">
@@ -3068,8 +3074,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B53" t="s">
@@ -3088,8 +3094,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54" s="2" t="s">
         <v>331</v>
       </c>
       <c r="B54" t="s">
@@ -3108,8 +3114,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55" s="2" t="s">
         <v>247</v>
       </c>
       <c r="B55" t="s">
@@ -3128,8 +3134,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56" s="2" t="s">
         <v>249</v>
       </c>
       <c r="B56" t="s">
@@ -3148,8 +3154,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57" s="2" t="s">
         <v>253</v>
       </c>
       <c r="B57" t="s">
@@ -3168,8 +3174,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B58" t="s">
@@ -3188,8 +3194,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59" s="2" t="s">
         <v>257</v>
       </c>
       <c r="B59" t="s">
@@ -3208,8 +3214,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" s="2" t="s">
         <v>259</v>
       </c>
       <c r="B60" t="s">
@@ -3228,8 +3234,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61" s="2" t="s">
         <v>261</v>
       </c>
       <c r="B61" t="s">
@@ -3248,8 +3254,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B62" t="s">
@@ -3268,8 +3274,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63" s="2" t="s">
         <v>263</v>
       </c>
       <c r="B63" t="s">
@@ -3288,8 +3294,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64" s="2" t="s">
         <v>265</v>
       </c>
       <c r="B64" t="s">
@@ -3308,8 +3314,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" s="2" t="s">
         <v>267</v>
       </c>
       <c r="B65" t="s">
@@ -3328,8 +3334,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B66" t="s">
@@ -3348,8 +3354,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" s="2" t="s">
         <v>270</v>
       </c>
       <c r="B67" t="s">
@@ -3368,8 +3374,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68" s="2" t="s">
         <v>272</v>
       </c>
       <c r="B68" t="s">
@@ -3388,8 +3394,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B69" t="s">
@@ -3408,8 +3414,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B70" t="s">
@@ -3428,8 +3434,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71" s="2" t="s">
         <v>279</v>
       </c>
       <c r="B71" t="s">
@@ -3448,8 +3454,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72" s="2" t="s">
         <v>324</v>
       </c>
       <c r="B72" t="s">
@@ -3468,8 +3474,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73" s="2" t="s">
         <v>276</v>
       </c>
       <c r="B73" t="s">
@@ -3488,8 +3494,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74" s="2" t="s">
         <v>281</v>
       </c>
       <c r="B74" t="s">
@@ -3508,8 +3514,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75" s="2" t="s">
         <v>283</v>
       </c>
       <c r="B75" t="s">
@@ -3528,8 +3534,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76" s="2" t="s">
         <v>326</v>
       </c>
       <c r="B76" t="s">
@@ -3548,8 +3554,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77" s="2" t="s">
         <v>285</v>
       </c>
       <c r="B77" t="s">
@@ -3568,8 +3574,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78" s="2" t="s">
         <v>287</v>
       </c>
       <c r="B78" t="s">
@@ -3588,8 +3594,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B79" t="s">
@@ -3608,8 +3614,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B80" t="s">
@@ -3628,8 +3634,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B81" t="s">
@@ -3648,8 +3654,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82" s="2" t="s">
         <v>293</v>
       </c>
       <c r="B82" t="s">
@@ -3668,8 +3674,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83" s="2" t="s">
         <v>339</v>
       </c>
       <c r="B83" t="s">
@@ -3688,8 +3694,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84" s="2" t="s">
         <v>289</v>
       </c>
       <c r="B84" t="s">
@@ -3708,8 +3714,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85" s="2" t="s">
         <v>291</v>
       </c>
       <c r="B85" t="s">
@@ -3728,8 +3734,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B86" t="s">
@@ -3748,8 +3754,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
         <v>237</v>
       </c>
       <c r="B87" t="s">
@@ -3768,8 +3774,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88" s="2" t="s">
         <v>295</v>
       </c>
       <c r="B88" t="s">
@@ -3788,8 +3794,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89" s="2" t="s">
         <v>297</v>
       </c>
       <c r="B89" t="s">
@@ -3808,8 +3814,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90" s="2" t="s">
         <v>299</v>
       </c>
       <c r="B90" t="s">
@@ -3828,8 +3834,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91" s="2" t="s">
         <v>251</v>
       </c>
       <c r="B91" t="s">
@@ -3848,8 +3854,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92" s="2" t="s">
         <v>277</v>
       </c>
       <c r="B92" t="s">
@@ -3868,8 +3874,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93" s="2" t="s">
         <v>278</v>
       </c>
       <c r="B93" t="s">
@@ -3888,8 +3894,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A94" s="2" t="s">
         <v>274</v>
       </c>
       <c r="B94" t="s">
@@ -3908,8 +3914,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A95" s="2" t="s">
         <v>306</v>
       </c>
       <c r="B95" t="s">
@@ -3928,8 +3934,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A96" s="2" t="s">
         <v>199</v>
       </c>
       <c r="B96" t="s">
@@ -3948,8 +3954,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A97" s="2" t="s">
         <v>205</v>
       </c>
       <c r="B97" t="s">
@@ -3968,8 +3974,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A98" s="2" t="s">
         <v>330</v>
       </c>
       <c r="B98" t="s">
@@ -3988,8 +3994,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A99" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B99" t="s">
@@ -4008,8 +4014,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100" s="2" t="s">
         <v>294</v>
       </c>
       <c r="B100" t="s">
@@ -4028,8 +4034,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101" s="2" t="s">
         <v>305</v>
       </c>
       <c r="B101" t="s">
@@ -4048,8 +4054,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A102" s="2" t="s">
         <v>447</v>
       </c>
       <c r="B102" t="s">
@@ -4068,8 +4074,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A103" s="2" t="s">
         <v>446</v>
       </c>
       <c r="B103" t="s">
@@ -4088,8 +4094,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104" s="2" t="s">
         <v>443</v>
       </c>
       <c r="B104" t="s">
@@ -4108,8 +4114,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A105" s="2" t="s">
         <v>445</v>
       </c>
       <c r="B105" t="s">
@@ -4128,8 +4134,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A106" s="2" t="s">
         <v>440</v>
       </c>
       <c r="B106" t="s">
@@ -4148,8 +4154,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B107" t="s">
@@ -4168,8 +4174,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B108" t="s">
@@ -4188,8 +4194,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B109" t="s">
@@ -4208,8 +4214,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A110" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B110" t="s">
@@ -4228,8 +4234,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A111" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B111" t="s">
@@ -4248,8 +4254,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B112" t="s">
@@ -4268,8 +4274,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A113" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B113" t="s">
@@ -4288,8 +4294,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A114" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B114" t="s">
@@ -4308,8 +4314,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A115" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B115" t="s">
@@ -4328,8 +4334,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A116" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B116" t="s">
@@ -4348,8 +4354,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B117" t="s">
@@ -4368,8 +4374,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A118" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B118" t="s">
@@ -4388,8 +4394,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A119" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B119" t="s">
@@ -4408,8 +4414,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B120" t="s">
@@ -4428,8 +4434,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B121" t="s">
@@ -4448,8 +4454,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A122" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B122" t="s">
@@ -4468,8 +4474,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A123" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B123" t="s">
@@ -4488,8 +4494,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A124" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B124" t="s">
@@ -4508,8 +4514,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A125" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B125" t="s">
@@ -4528,8 +4534,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A126" s="2" t="s">
         <v>428</v>
       </c>
       <c r="B126" t="s">
@@ -4548,8 +4554,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A127" s="2" t="s">
         <v>429</v>
       </c>
       <c r="B127" t="s">
@@ -4568,8 +4574,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A128" s="2" t="s">
         <v>430</v>
       </c>
       <c r="B128" t="s">
@@ -4588,8 +4594,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A129" s="2" t="s">
         <v>432</v>
       </c>
       <c r="B129" t="s">
@@ -4608,8 +4614,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A130" s="2" t="s">
         <v>434</v>
       </c>
       <c r="B130" t="s">
@@ -4628,8 +4634,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A131" s="2" t="s">
         <v>424</v>
       </c>
       <c r="B131" t="s">
@@ -4648,8 +4654,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A132" s="2" t="s">
         <v>436</v>
       </c>
       <c r="B132" t="s">
@@ -4668,8 +4674,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A133" s="2" t="s">
         <v>438</v>
       </c>
       <c r="B133" t="s">
@@ -4688,8 +4694,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A134" s="2" t="s">
         <v>437</v>
       </c>
       <c r="B134" t="s">
@@ -4708,8 +4714,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A135" s="2" t="s">
         <v>439</v>
       </c>
       <c r="B135" t="s">
@@ -4728,8 +4734,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A136" s="2" t="s">
         <v>406</v>
       </c>
       <c r="B136" t="s">
@@ -4748,8 +4754,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A137" s="2" t="s">
         <v>404</v>
       </c>
       <c r="B137" t="s">
@@ -4768,8 +4774,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A138" s="2" t="s">
         <v>359</v>
       </c>
       <c r="B138" t="s">
@@ -4788,8 +4794,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A139" s="2" t="s">
         <v>371</v>
       </c>
       <c r="B139" t="s">
@@ -4808,8 +4814,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A140" s="2" t="s">
         <v>409</v>
       </c>
       <c r="B140" t="s">
@@ -4828,8 +4834,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A141" s="2" t="s">
         <v>367</v>
       </c>
       <c r="B141" t="s">
@@ -4848,8 +4854,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A142" s="2" t="s">
         <v>358</v>
       </c>
       <c r="B142" t="s">
@@ -4868,8 +4874,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A143" s="2" t="s">
         <v>348</v>
       </c>
       <c r="B143" t="s">
@@ -4888,8 +4894,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A144" s="2" t="s">
         <v>351</v>
       </c>
       <c r="B144" t="s">
@@ -4908,8 +4914,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A145" s="2" t="s">
         <v>352</v>
       </c>
       <c r="B145" t="s">
@@ -4928,8 +4934,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A146" s="2" t="s">
         <v>372</v>
       </c>
       <c r="B146" t="s">
@@ -4948,8 +4954,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A147" s="2" t="s">
         <v>374</v>
       </c>
       <c r="B147" t="s">
@@ -4968,8 +4974,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A148" s="2" t="s">
         <v>408</v>
       </c>
       <c r="B148" t="s">
@@ -4988,8 +4994,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A149" s="2" t="s">
         <v>376</v>
       </c>
       <c r="B149" t="s">
@@ -5008,8 +5014,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A150" s="2" t="s">
         <v>378</v>
       </c>
       <c r="B150" t="s">
@@ -5028,8 +5034,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A151" s="2" t="s">
         <v>379</v>
       </c>
       <c r="B151" t="s">
@@ -5048,8 +5054,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A152" s="2" t="s">
         <v>383</v>
       </c>
       <c r="B152" t="s">
@@ -5068,8 +5074,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A153" s="2" t="s">
         <v>349</v>
       </c>
       <c r="B153" t="s">
@@ -5088,8 +5094,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A154" s="2" t="s">
         <v>384</v>
       </c>
       <c r="B154" t="s">
@@ -5108,8 +5114,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A155" s="2" t="s">
         <v>386</v>
       </c>
       <c r="B155" t="s">
@@ -5128,8 +5134,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A156" s="2" t="s">
         <v>344</v>
       </c>
       <c r="B156" t="s">
@@ -5148,8 +5154,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A157" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B157" t="s">
@@ -5168,8 +5174,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A158" s="2" t="s">
         <v>422</v>
       </c>
       <c r="B158" t="s">
@@ -5188,8 +5194,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A159" s="2" t="s">
         <v>416</v>
       </c>
       <c r="B159" t="s">
@@ -5208,8 +5214,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A160" s="2" t="s">
         <v>411</v>
       </c>
       <c r="B160" t="s">
@@ -5228,8 +5234,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A161" s="2" t="s">
         <v>388</v>
       </c>
       <c r="B161" t="s">
@@ -5248,8 +5254,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A162" s="2" t="s">
         <v>390</v>
       </c>
       <c r="B162" t="s">
@@ -5268,8 +5274,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A163" s="2" t="s">
         <v>392</v>
       </c>
       <c r="B163" t="s">
@@ -5288,8 +5294,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A164" s="2" t="s">
         <v>394</v>
       </c>
       <c r="B164" t="s">
@@ -5308,8 +5314,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A165" s="2" t="s">
         <v>396</v>
       </c>
       <c r="B165" t="s">
@@ -5328,8 +5334,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A166" s="2" t="s">
         <v>398</v>
       </c>
       <c r="B166" t="s">
@@ -5348,8 +5354,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A167" s="2" t="s">
         <v>414</v>
       </c>
       <c r="B167" t="s">
@@ -5368,8 +5374,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A168" s="2" t="s">
         <v>400</v>
       </c>
       <c r="B168" t="s">
@@ -5388,8 +5394,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A169" s="2" t="s">
         <v>363</v>
       </c>
       <c r="B169" t="s">
@@ -5408,8 +5414,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A170" s="2" t="s">
         <v>354</v>
       </c>
       <c r="B170" t="s">
@@ -5428,8 +5434,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A171" s="2" t="s">
         <v>356</v>
       </c>
       <c r="B171" t="s">
@@ -5448,8 +5454,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A172" s="2" t="s">
         <v>403</v>
       </c>
       <c r="B172" t="s">
@@ -5468,8 +5474,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A173" s="2" t="s">
         <v>413</v>
       </c>
       <c r="B173" t="s">
@@ -5488,8 +5494,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A174" s="2" t="s">
         <v>402</v>
       </c>
       <c r="B174" t="s">
@@ -5508,8 +5514,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A175" s="2" t="s">
         <v>365</v>
       </c>
       <c r="B175" t="s">
@@ -5528,8 +5534,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A176" s="2" t="s">
         <v>418</v>
       </c>
       <c r="B176" t="s">
@@ -5548,8 +5554,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A177" s="2" t="s">
         <v>361</v>
       </c>
       <c r="B177" t="s">
@@ -5568,8 +5574,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A178" s="2" t="s">
         <v>360</v>
       </c>
       <c r="B178" t="s">
@@ -5588,8 +5594,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A179" s="2" t="s">
         <v>381</v>
       </c>
       <c r="B179" t="s">
@@ -5608,8 +5614,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A180" s="2" t="s">
         <v>369</v>
       </c>
       <c r="B180" t="s">
@@ -5628,8 +5634,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A181" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B181" t="s">
@@ -5648,8 +5654,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A182" s="1" t="s">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A182" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B182" t="s">
@@ -5668,8 +5674,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A183" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B183" t="s">
@@ -5688,8 +5694,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="1" t="s">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A184" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B184" t="s">
@@ -5708,8 +5714,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="1" t="s">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A185" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B185" t="s">
@@ -5728,8 +5734,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="1" t="s">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A186" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B186" t="s">
@@ -5748,8 +5754,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A187" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B187" t="s">
@@ -5768,8 +5774,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A188" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B188" t="s">
@@ -5788,8 +5794,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A189" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B189" t="s">
@@ -5808,8 +5814,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A190" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B190" t="s">
@@ -5828,8 +5834,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A191" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B191" t="s">
@@ -5848,8 +5854,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A192" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B192" t="s">
@@ -5868,8 +5874,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A193" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B193" t="s">
@@ -5888,8 +5894,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A194" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B194" t="s">
@@ -5908,8 +5914,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A195" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B195" t="s">
@@ -5928,8 +5934,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A196" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B196" t="s">
@@ -5948,8 +5954,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="1" t="s">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A197" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B197" t="s">
@@ -5968,8 +5974,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A198" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B198" t="s">
@@ -5988,8 +5994,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A199" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B199" t="s">
@@ -6008,8 +6014,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A200" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B200" t="s">
@@ -6028,8 +6034,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A201" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B201" t="s">
@@ -6048,8 +6054,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A202" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B202" t="s">
@@ -6068,8 +6074,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A203" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B203" t="s">
@@ -6088,8 +6094,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A204" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B204" t="s">
@@ -6108,8 +6114,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" s="1" t="s">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A205" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B205" t="s">
@@ -6128,8 +6134,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A206" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B206" t="s">
@@ -6148,8 +6154,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A207" s="1" t="s">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A207" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B207" t="s">
@@ -6168,8 +6174,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208" s="1" t="s">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A208" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B208" t="s">
@@ -6188,8 +6194,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209" s="1" t="s">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A209" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B209" t="s">
@@ -6208,8 +6214,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" s="1" t="s">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A210" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B210" t="s">
@@ -6228,8 +6234,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" s="1" t="s">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A211" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B211" t="s">
@@ -6248,8 +6254,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="1" t="s">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A212" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B212" t="s">
@@ -6268,8 +6274,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="1" t="s">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A213" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B213" t="s">
@@ -6288,8 +6294,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="1" t="s">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A214" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B214" t="s">
@@ -6308,8 +6314,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="1" t="s">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A215" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B215" t="s">
@@ -6328,8 +6334,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="1" t="s">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A216" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B216" t="s">
@@ -6348,8 +6354,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="1" t="s">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A217" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B217" t="s">
@@ -6368,8 +6374,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="1" t="s">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A218" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B218" t="s">
@@ -6388,8 +6394,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="1" t="s">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A219" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B219" t="s">
@@ -6408,8 +6414,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="1" t="s">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A220" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B220" t="s">
@@ -6428,8 +6434,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A221" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B221" t="s">
@@ -6448,8 +6454,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A222" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B222" t="s">
@@ -6468,8 +6474,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="1" t="s">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A223" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B223" t="s">
@@ -6488,8 +6494,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A224" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B224" t="s">
@@ -6508,8 +6514,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A225" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B225" t="s">
@@ -6528,8 +6534,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="1" t="s">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A226" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B226" t="s">
@@ -6548,8 +6554,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A227" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B227" t="s">
@@ -6568,8 +6574,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="1" t="s">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A228" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B228" t="s">
@@ -6588,8 +6594,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A229" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B229" t="s">
@@ -6608,8 +6614,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A230" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B230" t="s">
@@ -6628,8 +6634,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A231" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B231" t="s">
@@ -6648,8 +6654,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A232" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B232" t="s">
@@ -6668,8 +6674,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A233" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B233" t="s">
@@ -6688,8 +6694,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A234" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B234" t="s">
@@ -6708,8 +6714,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A235" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B235" t="s">
@@ -6728,8 +6734,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A236" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B236" t="s">
@@ -6748,8 +6754,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A237" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B237" t="s">
@@ -6768,8 +6774,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A238" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B238" t="s">
@@ -6788,8 +6794,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A239" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B239" t="s">
@@ -6808,8 +6814,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A240" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B240" t="s">
@@ -6828,8 +6834,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A241" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B241" t="s">
@@ -6848,8 +6854,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A242" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B242" t="s">
@@ -6868,8 +6874,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A243" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B243" t="s">
@@ -6888,8 +6894,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A244" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B244" t="s">
@@ -6908,8 +6914,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A245" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B245" t="s">
@@ -6928,8 +6934,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A246" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B246" t="s">
@@ -6948,8 +6954,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A247" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B247" t="s">
@@ -6968,8 +6974,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A248" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B248" t="s">
@@ -6988,8 +6994,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A249" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B249" t="s">
@@ -7008,8 +7014,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A250" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B250" t="s">
@@ -7028,8 +7034,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A251" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B251" t="s">
@@ -7048,8 +7054,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A252" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B252" t="s">
@@ -7071,5 +7077,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>